<commit_message>
PySpark RDD Basic Actions uygulama eklendi
</commit_message>
<xml_diff>
--- a/docs/rdd_transformations_aggregate_iterasyon_sema.xlsx
+++ b/docs/rdd_transformations_aggregate_iterasyon_sema.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22365" windowHeight="10020"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet name="scala" sheetId="1" r:id="rId1"/>
+    <sheet name="python" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>x._1</t>
   </si>
@@ -72,6 +73,24 @@
   </si>
   <si>
     <t>(49,3)</t>
+  </si>
+  <si>
+    <t>(lambda x,y: (x[0] + y, x[0] + 1)</t>
+  </si>
+  <si>
+    <t>x[0]</t>
+  </si>
+  <si>
+    <t>x[1]</t>
+  </si>
+  <si>
+    <t>(lambdax,y: (x[0] + y[0], x[1] + y[1])</t>
+  </si>
+  <si>
+    <t>y[0]</t>
+  </si>
+  <si>
+    <t>y[1]</t>
   </si>
 </sst>
 </file>
@@ -192,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -228,17 +247,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,7 +545,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:Q10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,69 +554,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
     </row>
     <row r="2" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
     </row>
     <row r="3" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="G3" s="15" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="G3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="M3" s="15" t="s">
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="M3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
     </row>
     <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -806,56 +828,56 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
     </row>
     <row r="11" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
     </row>
     <row r="12" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
     </row>
     <row r="14" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G14" s="1" t="s">
@@ -953,4 +975,438 @@
     <ignoredError sqref="G16:G17" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="17" width="6.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+    </row>
+    <row r="2" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+    </row>
+    <row r="3" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="G3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="M3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+    </row>
+    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="13">
+        <v>9</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>9</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>1</v>
+      </c>
+      <c r="M5" s="13">
+        <v>5</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6">
+        <v>5</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="13">
+        <v>4</v>
+      </c>
+      <c r="H6" s="5">
+        <v>9</v>
+      </c>
+      <c r="I6" s="6">
+        <v>4</v>
+      </c>
+      <c r="J6" s="5">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="13">
+        <v>36</v>
+      </c>
+      <c r="N6" s="5">
+        <v>5</v>
+      </c>
+      <c r="O6" s="6">
+        <v>36</v>
+      </c>
+      <c r="P6" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>3</v>
+      </c>
+      <c r="B7" s="7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="13">
+        <v>10</v>
+      </c>
+      <c r="H7" s="7">
+        <v>13</v>
+      </c>
+      <c r="I7" s="8">
+        <v>10</v>
+      </c>
+      <c r="J7" s="7">
+        <v>2</v>
+      </c>
+      <c r="K7" s="8">
+        <v>1</v>
+      </c>
+      <c r="M7" s="13">
+        <v>8</v>
+      </c>
+      <c r="N7" s="7">
+        <v>41</v>
+      </c>
+      <c r="O7" s="8">
+        <v>8</v>
+      </c>
+      <c r="P7" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="9">
+        <v>6</v>
+      </c>
+      <c r="E9" s="9">
+        <v>3</v>
+      </c>
+      <c r="I9" s="9">
+        <v>23</v>
+      </c>
+      <c r="K9" s="9">
+        <v>3</v>
+      </c>
+      <c r="O9" s="9">
+        <v>49</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+    </row>
+    <row r="11" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+    </row>
+    <row r="12" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6">
+        <v>6</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0</v>
+      </c>
+      <c r="K15" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="5">
+        <v>6</v>
+      </c>
+      <c r="I16" s="6">
+        <v>23</v>
+      </c>
+      <c r="J16" s="5">
+        <v>3</v>
+      </c>
+      <c r="K16" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="7:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="7">
+        <v>29</v>
+      </c>
+      <c r="I17" s="8">
+        <v>49</v>
+      </c>
+      <c r="J17" s="7">
+        <v>6</v>
+      </c>
+      <c r="K17" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="7:11" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="7:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I19" s="11">
+        <v>78</v>
+      </c>
+      <c r="J19" s="12"/>
+      <c r="K19" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="7:11" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A11:Q11"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="A10:Q10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>